<commit_message>
bulk email and evalreg
</commit_message>
<xml_diff>
--- a/src/assets/img/sampleFile.xlsx
+++ b/src/assets/img/sampleFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Medha Office\Projects\Sim-FE-2025\src\assets\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EE60489-02CD-4B9B-BC4D-166C30385D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53640811-E739-415F-BAE3-440D827AFEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2929A569-DA4F-41D7-A512-8897FD3F9E10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>full_name</t>
   </si>
@@ -56,19 +56,34 @@
     <t>ddsxzcvxzc</t>
   </si>
   <si>
-    <t>xzcvcxv</t>
-  </si>
-  <si>
-    <t>verbvfbgf</t>
-  </si>
-  <si>
     <t>fbvcbvc@gmail.com</t>
   </si>
   <si>
-    <t>dsbrtebre@gmail.com</t>
-  </si>
-  <si>
-    <t>jhythjy@gmail.com</t>
+    <t>state</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>English,Hindi-हिन्दी,Kannada-ಕೆನಡಾ,Malayalam-മലയാളം,Other Language,Tamil-தமிழ்,Telugu-తెలుగు</t>
+  </si>
+  <si>
+    <t>Sustainable Development and Environment,Digital Transformation,Health and Well-being,Quality Education,Economic Empowerment,Smart and Resilient Communities,Agriculture and Rural Development,Others</t>
+  </si>
+  <si>
+    <t>Andaman and Nicobar Islands,Andhra Pradesh,Arunachal Pradesh,Assam,Bihar,Chandigarh,Chhattisgarh,Dadra and Nagar Haveli and Daman and Diu,Delhi,Goa,Gujarat,Haryana,Himachal Pradesh,Jammu and Kashmir,Jharkhand,Karnataka,Kerala,Ladakh,Lakshadweep,Madhya Pradesh,Maharashtra,Manipur,Meghalaya,Mizoram,Nagaland,Odisha,Puducherry,Punjab,Rajasthan,Sikkim,Tamil Nadu,Telangana,Tripura,Uttar Pradesh,Uttarakhand,West Bengal</t>
+  </si>
+  <si>
+    <t>Meghalaya,Mizoram,Nagaland,Sikkim,Tamil Nadu,Telangana,Tripura,Uttar Pradesh,Uttarakhand,West Bengal</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Health and Well-being,Quality Education</t>
   </si>
 </sst>
 </file>
@@ -451,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95B7C0A-8667-40AB-83F4-7BDAA78C8BE4}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +477,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +487,17 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -483,46 +507,46 @@
       <c r="C2">
         <v>214325325</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>21325436</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>676585</v>
-      </c>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>547658</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2C488072-79A2-48E8-8837-14D7A65A4FDE}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{B2C26EF7-EAC3-40C2-A96C-FE71BF16FB9B}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{4649406B-58E6-4AF1-AB63-4A24CA41AC02}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{09A89463-2D02-4840-A95F-9FE84D6622CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>